<commit_message>
fine tune the intents, save report function
</commit_message>
<xml_diff>
--- a/rasaproject8/interface/user_data.xlsx
+++ b/rasaproject8/interface/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,27 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>phone_number</t>
+          <t>phoneNumber</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>phone_number2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>router_status</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>phone_status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Instrument_status</t>
+          <t>issue</t>
         </is>
       </c>
     </row>
@@ -477,21 +462,6 @@
         </is>
       </c>
       <c r="C2" t="inlineStr">
-        <is>
-          <t>0987654321</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Online</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
         <is>
           <t>Working</t>
         </is>

</xml_diff>